<commit_message>
added days 3 and 4
</commit_message>
<xml_diff>
--- a/Day 1/Transactions.xlsx
+++ b/Day 1/Transactions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maldonadocz-my.sharepoint.com/personal/pablo_maldonado_cz/Documents/TRAINING/CLIENTS/NOBLEPROG/uipath/uipath4daycourse/Day 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Desktop\np-uipath-starter\Day 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{5A250F64-3D13-4B75-BA35-C64637A692A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51DFF451-82E8-4EC3-8E1F-18CB89F76524}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46083CF3-E73C-4E87-BE67-F344561D641B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{51FEC241-2751-4292-AE37-BDE7C5C99299}"/>
+    <workbookView xWindow="-24945" yWindow="2580" windowWidth="21600" windowHeight="11295" xr2:uid="{51FEC241-2751-4292-AE37-BDE7C5C99299}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -444,6 +444,9 @@
       <c r="C2">
         <v>90</v>
       </c>
+      <c r="D2">
+        <v>138514</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -455,6 +458,9 @@
       <c r="C3">
         <v>465</v>
       </c>
+      <c r="D3">
+        <v>138515</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -465,6 +471,9 @@
       </c>
       <c r="C4">
         <v>620</v>
+      </c>
+      <c r="D4">
+        <v>138516</v>
       </c>
     </row>
   </sheetData>

</xml_diff>